<commit_message>
Finalizada la Activity para crear una receta, persistencia correcta.
</commit_message>
<xml_diff>
--- a/material/Webgrafía.xlsx
+++ b/material/Webgrafía.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isra\AndroidStudioProjects\RecetasDigitales\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4179157B-C479-4066-BA4C-D75F7D88BF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE35FB7-B916-466C-A789-DD010F7B10D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44101532-F571-4096-951B-078E0E9D855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44101532-F571-4096-951B-078E0E9D855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -346,132 +346,28 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color theme="7"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="medium">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="7"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -499,31 +395,135 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
+      <border>
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
         <top style="medium">
-          <color indexed="64"/>
+          <color theme="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="7"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Webgrafia" pivot="0" count="9" xr9:uid="{F6F4BA48-2D36-4345-8CCC-7DD8EFB7F428}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstColumn" dxfId="7"/>
-      <tableStyleElement type="lastColumn" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondRowStripe" dxfId="4"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="3"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -538,14 +538,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E7B9A33-2B30-47FB-847B-B298BBF0A426}" name="Tabla1" displayName="Tabla1" ref="A1:B58" totalsRowCount="1" headerRowDxfId="14" dataDxfId="11" headerRowBorderDxfId="15" tableBorderDxfId="16">
-  <autoFilter ref="A1:B57" xr:uid="{4E7B9A33-2B30-47FB-847B-B298BBF0A426}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E7B9A33-2B30-47FB-847B-B298BBF0A426}" name="Tabla1" displayName="Tabla1" ref="A1:B59" totalsRowCount="1" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A1:B58" xr:uid="{4E7B9A33-2B30-47FB-847B-B298BBF0A426}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FAED532A-6363-46FB-9118-4D87FCEA4634}" name="URL" dataDxfId="13" totalsRowDxfId="1" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="2" xr3:uid="{87D96FBE-5A90-42F4-B9AB-4ED2310095A1}" name="Fecha" dataDxfId="12" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FAED532A-6363-46FB-9118-4D87FCEA4634}" name="URL" dataDxfId="3" totalsRowDxfId="1" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="2" xr3:uid="{87D96FBE-5A90-42F4-B9AB-4ED2310095A1}" name="Fecha" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Webgrafia" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -868,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717859A7-562F-4C5B-AEFA-28975BE776C0}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,8 +1337,12 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Refactorizacion del VerRecetasAdapter y Holder. Añadimos el atributo android:windowSoftInputMode="adjustPan" a la Activity VerRecetas del AndroidManifest.xml, esto evita que el fondo se redimensione ya que tiene bastante impacto visual
</commit_message>
<xml_diff>
--- a/material/Webgrafía.xlsx
+++ b/material/Webgrafía.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isra\AndroidStudioProjects\RecetasDigitales\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE35FB7-B916-466C-A789-DD010F7B10D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12F0FA2-9B58-4EE3-82D7-F9CAAD6EBE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44101532-F571-4096-951B-078E0E9D855C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>URL</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>https://developer.android.com/reference/android/graphics/drawable/StateListDrawable</t>
+  </si>
+  <si>
+    <t>https://medium.com/@kumargaurav.xqf/mastering-recyclerview-optimizing-oncreateviewholder-and-onbindviewholder-for-large-datasets-a05d9249a1b1</t>
   </si>
 </sst>
 </file>
@@ -871,12 +874,12 @@
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="115.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="139.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1337,8 +1340,12 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="5">
+        <v>45970</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>

</xml_diff>